<commit_message>
working out assay definitions
</commit_message>
<xml_diff>
--- a/isatools/net/resources/mtbls/StudyTerms4Curators-template.xlsx
+++ b/isatools/net/resources/mtbls/StudyTerms4Curators-template.xlsx
@@ -1,21 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10914"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philippe/Documents/git/isa-api2/isa-api/isatools/net/resources/mtbls/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945C51FA-C766-7E4D-803B-46D875ACBFE9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23947399-72CE-F845-923F-40FE4C1E8B0B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3580" yWindow="2560" windowWidth="27240" windowHeight="16440" activeTab="2" xr2:uid="{706403F5-489F-AD48-8BF2-F3744C7F4E3A}"/>
+    <workbookView xWindow="3580" yWindow="2560" windowWidth="27240" windowHeight="16440" firstSheet="1" activeTab="10" xr2:uid="{706403F5-489F-AD48-8BF2-F3744C7F4E3A}"/>
   </bookViews>
   <sheets>
     <sheet name="GC-MS Study" sheetId="1" r:id="rId1"/>
     <sheet name="LC-MS Study" sheetId="2" r:id="rId2"/>
     <sheet name="NMR Study" sheetId="3" r:id="rId3"/>
+    <sheet name="CE-MS Study" sheetId="4" r:id="rId4"/>
+    <sheet name="SPE-IMS-MS Study" sheetId="5" r:id="rId5"/>
+    <sheet name="DI-MS Study" sheetId="6" r:id="rId6"/>
+    <sheet name="Imaging-MS Study" sheetId="9" r:id="rId7"/>
+    <sheet name="MALDI-MS Study" sheetId="8" r:id="rId8"/>
+    <sheet name="FIA-MS Study" sheetId="7" r:id="rId9"/>
+    <sheet name="GCxGC-MS Study" sheetId="10" r:id="rId10"/>
+    <sheet name="LC-DAD Study" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="550">
   <si>
     <t>Parameter Value[Chromatography Instrument]</t>
   </si>
@@ -1494,6 +1502,189 @@
   </si>
   <si>
     <t>Parameter Value[NMR Pulse Sequence Name]</t>
+  </si>
+  <si>
+    <t>Agilent 1100 Series Isocratic Pump, G1603A CE-MS Adapter Kit, and G1607A CE-ESI-MS Sprayer Kit</t>
+  </si>
+  <si>
+    <t>CE bare fused-silica capillary (50 μm x 800 mm; Agilent Technologies)</t>
+  </si>
+  <si>
+    <t>Agilent 1600A Capillary Electrophoresis, Agilent 1100 Series Isocratic Pump, and G1607A CE-ESI-MS Sprayer Kit</t>
+  </si>
+  <si>
+    <t>CE bare fused-silica capillary (50 μm x 1,000 mm; Agilent Technologies)</t>
+  </si>
+  <si>
+    <t>Agilent 7100 CE System</t>
+  </si>
+  <si>
+    <t>Parameter Value[Cartridge type]</t>
+  </si>
+  <si>
+    <t>Agilent RapidFire 365</t>
+  </si>
+  <si>
+    <t>C18</t>
+  </si>
+  <si>
+    <t>mixed mode</t>
+  </si>
+  <si>
+    <t>graphitic carbon</t>
+  </si>
+  <si>
+    <t>Parameter Value[Instrument]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Ion source]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Mass analyzer]</t>
+  </si>
+  <si>
+    <t>AB SCIEX 4800 Plus MALDI TOF/TOF</t>
+  </si>
+  <si>
+    <t>MS:matrix-assisted laser desorption ionization</t>
+  </si>
+  <si>
+    <t>MS:time-of-flight</t>
+  </si>
+  <si>
+    <t>AB SCIEX TOF/TOF 5800</t>
+  </si>
+  <si>
+    <t>Bruker ultrafleXtreme</t>
+  </si>
+  <si>
+    <t>Parameter Value[Sample mounting]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Sample preservation]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Sectioning instrument]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Line scan direction]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Line scan sequence]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Scan pattern]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Scan type]</t>
+  </si>
+  <si>
+    <t>Glass slide</t>
+  </si>
+  <si>
+    <t>Fresh frozen</t>
+  </si>
+  <si>
+    <t>Thermo Scientific Shandon Cryotome</t>
+  </si>
+  <si>
+    <t>Bruker solariX XR</t>
+  </si>
+  <si>
+    <t>MS:electrospray ionization</t>
+  </si>
+  <si>
+    <t>Hybrid Qh-FTMS</t>
+  </si>
+  <si>
+    <t>linescan left right</t>
+  </si>
+  <si>
+    <t>top down</t>
+  </si>
+  <si>
+    <t>flyback</t>
+  </si>
+  <si>
+    <t>horizontal</t>
+  </si>
+  <si>
+    <t>Thermo Scientific X72 SuperFrost Plus Adhesion slide</t>
+  </si>
+  <si>
+    <t>Thermo Scientific Microm HM550 Cryostat</t>
+  </si>
+  <si>
+    <t>Thermo Scientific LTQ Orbitrap XL ETD</t>
+  </si>
+  <si>
+    <t>MS:orbitrap</t>
+  </si>
+  <si>
+    <t>Thermo Scientific FB58628 Fisherbrand Glass slide</t>
+  </si>
+  <si>
+    <t>Leica CM3050 S</t>
+  </si>
+  <si>
+    <t>Thermo Scientific MALDI LTQ Orbitrap XL</t>
+  </si>
+  <si>
+    <t>Thermo Scientific SuperFrost Glass slide</t>
+  </si>
+  <si>
+    <t>Thermo Scientific MALDI LTQ Orbitrap Discovery</t>
+  </si>
+  <si>
+    <t>Delta Electronics ITO one surface glass slide</t>
+  </si>
+  <si>
+    <t>Thermo Scientific Orbitrap Elite</t>
+  </si>
+  <si>
+    <t>Thermo Scientific Polysine Adhesion Slide</t>
+  </si>
+  <si>
+    <t>Parameter Value[Detector]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Signal range]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Resolution]</t>
+  </si>
+  <si>
+    <t>Waters ACQUITY UPLC PDA Detector</t>
+  </si>
+  <si>
+    <t>190-500 nm</t>
+  </si>
+  <si>
+    <t>0.25 nm</t>
+  </si>
+  <si>
+    <t>210-450 nm</t>
+  </si>
+  <si>
+    <t>2 nm</t>
+  </si>
+  <si>
+    <t>Waters ACQUITY UPLC PDA eλ Detector</t>
+  </si>
+  <si>
+    <t>250-600 nm</t>
+  </si>
+  <si>
+    <t>1.2 nm</t>
+  </si>
+  <si>
+    <t>Agilent 1290 Infinity DAD Detector</t>
+  </si>
+  <si>
+    <t>200-600 nm</t>
+  </si>
+  <si>
+    <t>1 nm</t>
   </si>
 </sst>
 </file>
@@ -2421,11 +2612,95 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48F42706-BBA6-6340-8287-CCB83055A864}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S34" sqref="S34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{262F0CC3-9E7A-E946-99D9-660EE4DEAE71}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q29" sqref="Q29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>539</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>544</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>547</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>549</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48467566-1CAC-7F4D-AEFD-016885F11A7F}">
   <dimension ref="A1:C142"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
@@ -3846,7 +4121,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D450F36E-855A-3542-AFDF-1AFE50D8F16E}">
   <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -5163,4 +5438,411 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F27BF470-234E-A54E-A2D4-63A6EB74AA0A}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{340E4251-B341-B540-8F6F-482CD4DE5D0F}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
+      <c r="B3" s="2" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="4"/>
+      <c r="B4" s="2" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="4"/>
+      <c r="B5" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3051137-0B0D-EE4D-8776-BB65E14B587E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{756AE5CB-9135-7142-88DA-610FD139EFE0}">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="K1" s="4"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>518</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="K2" s="4"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>503</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E917EFD-3D3C-D04C-A508-7FC0B47CB7A6}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCellId="1" sqref="A1:C4 A1:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FFCB201-DE10-DC4E-839A-0EC6C658A54A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P27" sqref="P27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>